<commit_message>
Update workflow and Fixed rate_list item detail
</commit_message>
<xml_diff>
--- a/rate_list.xlsx
+++ b/rate_list.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\New folder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\ext_proj Grocery Store\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -604,8 +604,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E79"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1026,10 +1026,10 @@
         <v>19</v>
       </c>
       <c r="C25">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="D25" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E25">
         <v>8</v>

</xml_diff>